<commit_message>
Queries 21 a 24
</commit_message>
<xml_diff>
--- a/src/site/sf110_semantic_v1.xlsx
+++ b/src/site/sf110_semantic_v1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="9555" windowHeight="7755" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="9555" windowHeight="7755" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="SQL DDL" sheetId="30" r:id="rId1"/>
@@ -23,17 +23,18 @@
     <sheet name="R5" sheetId="20" r:id="rId9"/>
     <sheet name="R6" sheetId="25" r:id="rId10"/>
     <sheet name="R7" sheetId="36" r:id="rId11"/>
+    <sheet name="R8" sheetId="37" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'R5'!$B$98:$E$98</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'R6'!$B$4:$O$4</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1810" uniqueCount="804">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2364" uniqueCount="939">
   <si>
     <t>boolean</t>
   </si>
@@ -2445,12 +2446,417 @@
   </si>
   <si>
     <t>t    = expandTypes;                  // True: Considera com Expansão de Tipos para o Retorno e Parâmetros | False: Mesmos Retorno e Parâmetros</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- v_interface_metrics_pairs</t>
+  </si>
+  <si>
+    <t>DROP view IF EXISTS v_interface_metrics_pairs;</t>
+  </si>
+  <si>
+    <t>CREATE view v_interface_metrics_pairs as</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       a.project_name a_project_name,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       a.entity_id a_entity_id,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       a.id a_id,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       concat(a.modifiers,' ',a.return_type, ' ', a.fqn, a.params) a_fqn,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       concat(b.modifiers,' ',b.return_type, ' ', b.fqn, b.params) b_fqn,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       b.id b_id,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       b.entity_id b_entity_id,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       b.project_name b_project_name,</t>
+  </si>
+  <si>
+    <t>and    b.id = p.interface_metrics_b;</t>
+  </si>
+  <si>
+    <t>select p.search_type,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">       ((CASE WHEN a.result1 = b.result1 THEN 1 else 0 END) +</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        (CASE WHEN a.result2 = b.result2 THEN 1 else 0 END) +</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        (CASE WHEN a.result3 = b.result3 THEN 1 else 0 END)) as 'semantic',</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       a.project_id a_project_id,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       b.project_id b_project_id,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       a.result1 a_result1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       a.result2 a_result2,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       a.result3 a_result3,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       a.exec1 a_exec1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       a.exec2 a_exec2,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       a.exec3 a_exec3,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       a.error a_error,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       b.result1 b_result1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       b.result2 b_result2,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       b.result3 b_result3,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       b.exec1 b_exec1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       b.exec2 b_exec2,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       b.exec3 b_exec3,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       b.error b_error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       a.project_type a_project_type,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       b.project_type b_project_type,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       p.compare_result,</t>
+  </si>
+  <si>
+    <t>DROP view IF EXISTS v_interface_metrics_compare;</t>
+  </si>
+  <si>
+    <t>CREATE view v_interface_metrics_compare as</t>
+  </si>
+  <si>
+    <t>select c.type,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       c.result,</t>
+  </si>
+  <si>
+    <t>from   interface_metrics_compare c,</t>
+  </si>
+  <si>
+    <t>where  a.id = c.interface_metrics_a</t>
+  </si>
+  <si>
+    <t>and    b.id = c.interface_metrics_b;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- v_interface_metrics_compare</t>
+  </si>
+  <si>
+    <t>/*</t>
+  </si>
+  <si>
+    <t>-&gt; sf110_semantic_v1.xlsx</t>
+  </si>
+  <si>
+    <t>p = differentPackage; // True: Ignora os packages | False: Mesmos packages</t>
+  </si>
+  <si>
+    <t>c = ignoreClass;      // True: Ignora as Classes | False: Considera com Expansão Wordnet</t>
+  </si>
+  <si>
+    <t>w = expandMethodName; // True: Considera com Expansão Wordnet | False: Mesmos nomes de Métodos</t>
+  </si>
+  <si>
+    <t>t = expandTypes;      // True: Considera com Expansão de Tipos para o Retorno e Parâmetros | False: Mesmos Retorno e Parâmetros</t>
+  </si>
+  <si>
+    <t>*/</t>
+  </si>
+  <si>
+    <t>select '(1) Número de pares de métodos com interface similar s/ considerar o nome da classe' description, count(*) total</t>
+  </si>
+  <si>
+    <t>from   v_interface_metrics_pairs</t>
+  </si>
+  <si>
+    <t>where  search_type = 'p1_c1_w1_t1'</t>
+  </si>
+  <si>
+    <t>UNION all</t>
+  </si>
+  <si>
+    <t>from   v_interface_metrics_compare</t>
+  </si>
+  <si>
+    <t>where  type = 'p1_c1_w1_t1'</t>
+  </si>
+  <si>
+    <t>and    result = 3</t>
+  </si>
+  <si>
+    <t>and    result = 2</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> #21 SCAM 2017</t>
+  </si>
+  <si>
+    <t>select '  (1.a) Para quantos desses batem as três saídas para as três entradas (redundantes)' description, count(*) total</t>
+  </si>
+  <si>
+    <t>select '  (1.b) Para quantos desses batem duas saídas para as três entradas' description, count(*) total</t>
+  </si>
+  <si>
+    <t>select '(2) Número de pares de métodos com interface similar considerando o nome da classe' description, count(*) total</t>
+  </si>
+  <si>
+    <t>where  search_type = 'p1_c0_w1_t1'</t>
+  </si>
+  <si>
+    <t>select '  (2.a) Para quantos desses batem as três saídas para as três entradas (redundantes)' description, count(*) total</t>
+  </si>
+  <si>
+    <t>where  type = 'p1_c0_w1_t1'</t>
+  </si>
+  <si>
+    <t>select '  (2.b) Para quantos desses batem duas saídas para as três entradas' description, count(*) total</t>
+  </si>
+  <si>
+    <t>select '(3) Qual é o número de métodos considerados no experimento (que casam com o filtro - estático, só tipos primitivos, etc.)?' description, count(*) total</t>
+  </si>
+  <si>
+    <t>from   interface_metrics i</t>
+  </si>
+  <si>
+    <t>where  return_type in (select type from interface_metrics_types where class in (1, 2, 3))</t>
+  </si>
+  <si>
+    <t>and    id in (</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               select interface_metrics_id from interface_metrics_params</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               where  param in (select type from interface_metrics_types where class in (1, 2, 3))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">               and    interface_metrics_id = i.id</t>
+  </si>
+  <si>
+    <t>and project_type = 'CRAWLED'</t>
+  </si>
+  <si>
+    <t>select '(4) Qual é o número de projetos considerados no experimento (que contém pelo menos um método que casa com o filtro - estático, só tipos primitivos, etc.)?' description, count(proj) total</t>
+  </si>
+  <si>
+    <t>select count(*) proj</t>
+  </si>
+  <si>
+    <t>and    project_type = 'CRAWLED'</t>
+  </si>
+  <si>
+    <t>GROUP BY project_id</t>
+  </si>
+  <si>
+    <t>) t</t>
+  </si>
+  <si>
+    <t>select '(7) Qual é o número de métodos redundantes (para os quais existe pelo menos outro método semelhante no qual batem as três saídas para as três entradas)?' description, count(*) total</t>
+  </si>
+  <si>
+    <t>select distinct a_id</t>
+  </si>
+  <si>
+    <t>where  result = 3</t>
+  </si>
+  <si>
+    <t>and    type = 'p1_c1_w1_t1'</t>
+  </si>
+  <si>
+    <t>) as t</t>
+  </si>
+  <si>
+    <t>select '(8) Qual é o número de projetos que contém pelo menos um método redundante (método para o qual existe pelo menos outro método semelhante no qual batem as três saídas para as três entradas)' description, count(*) total</t>
+  </si>
+  <si>
+    <t>select a_project_id</t>
+  </si>
+  <si>
+    <t>group by a_project_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- #22 SCAM 2017</t>
+  </si>
+  <si>
+    <t>select project_type, project_id, project_name, count(*)</t>
+  </si>
+  <si>
+    <t>GROUP BY project_type, project_id, project_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- #23 SCAM 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- (6) Qual é o número de métodos no experimento que são redundantes (batem as três saídas para as três entradas) por projeto?</t>
+  </si>
+  <si>
+    <t>select a_project_type, a_project_id, a_project_name, count(*), result</t>
+  </si>
+  <si>
+    <t>GROUP BY a_project_type, a_project_id, a_project_name, result</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- #24 SCAM 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- (9) Quais são os pares crawled-crawled para os quais batem as três saídas para as três entradas?</t>
+  </si>
+  <si>
+    <t>select *</t>
+  </si>
+  <si>
+    <t>and    b_project_type = 'CRAWLED'</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>(1) Número de pares de métodos com interface similar s/ considerar o nome da classe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (1.a) Para quantos desses batem as três saídas para as três entradas (redundantes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (1.b) Para quantos desses batem duas saídas para as três entradas</t>
+  </si>
+  <si>
+    <t>(2) Número de pares de métodos com interface similar considerando o nome da classe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (2.a) Para quantos desses batem as três saídas para as três entradas (redundantes)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  (2.b) Para quantos desses batem duas saídas para as três entradas</t>
+  </si>
+  <si>
+    <t>(3) Qual é o número de métodos considerados no experimento (que casam com o filtro - estático, só tipos primitivos, etc.)?</t>
+  </si>
+  <si>
+    <t>(4) Qual é o número de projetos considerados no experimento (que contém pelo menos um método que casa com o filtro - estático, só tipos primitivos, etc.)?</t>
+  </si>
+  <si>
+    <t>(7) Qual é o número de métodos redundantes (para os quais existe pelo menos outro método semelhante no qual batem as três saídas para as três entradas)?</t>
+  </si>
+  <si>
+    <t>(8) Qual é o número de projetos que contém pelo menos um método redundante (método para o qual existe pelo menos outro método semelhante no qual batem as três saídas para as três entradas)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- #21 SCAM 2017</t>
+  </si>
+  <si>
+    <t>count(*)</t>
+  </si>
+  <si>
+    <t>a_project_type</t>
+  </si>
+  <si>
+    <t>a_project_id</t>
+  </si>
+  <si>
+    <t>a_project_name</t>
+  </si>
+  <si>
+    <t>result</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -- (5) Qual é o número de métodos considerados no experimento por projeto?</t>
+  </si>
+  <si>
+    <t>p1_c1_w1_t1</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>a_entity_id</t>
+  </si>
+  <si>
+    <t>a_id</t>
+  </si>
+  <si>
+    <t>a_fqn</t>
+  </si>
+  <si>
+    <t>b_fqn</t>
+  </si>
+  <si>
+    <t>b_id</t>
+  </si>
+  <si>
+    <t>b_entity_id</t>
+  </si>
+  <si>
+    <t>b_project_name</t>
+  </si>
+  <si>
+    <t>b_project_id</t>
+  </si>
+  <si>
+    <t>b_project_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       c.exec1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       c.exec2,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       c.exec3</t>
+  </si>
+  <si>
+    <t>exec1</t>
+  </si>
+  <si>
+    <t>exec2</t>
+  </si>
+  <si>
+    <t>exec3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
@@ -3710,7 +4116,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3748,7 +4154,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3783,6 +4189,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3818,9 +4241,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3997,7 +4437,7 @@
   <dimension ref="A2:B284"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A50" sqref="A5:A50"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9705,7 +10145,7 @@
   <dimension ref="B1:T32"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11511,12 +11951,2633 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="8" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="B1:W71"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.625" style="120" customWidth="1"/>
+    <col min="2" max="2" width="30.75" style="120" customWidth="1"/>
+    <col min="3" max="3" width="10.625" style="120" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.25" style="120" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.875" style="120" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.625" style="120" customWidth="1"/>
+    <col min="7" max="7" width="57.25" style="120" customWidth="1"/>
+    <col min="8" max="8" width="12.75" style="120" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.25" style="120" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.75" style="120" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.25" style="120" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.375" style="120" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.5" style="120" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="92.25" style="120" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="104.375" style="120" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.5" style="120" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.375" style="120" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.25" style="120" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.75" style="120" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.125" style="120" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.375" style="120" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="6.75" style="120" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.125" style="120" customWidth="1"/>
+    <col min="25" max="16384" width="9" style="120"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>921</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>915</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>916</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>904</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>863</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1487</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>637</v>
+      </c>
+      <c r="E4" s="6">
+        <v>5</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>905</v>
+      </c>
+      <c r="H4" s="7">
+        <v>39299</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="6">
+        <v>1488</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="E5" s="6">
+        <v>135</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>906</v>
+      </c>
+      <c r="H5" s="7">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1489</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>659</v>
+      </c>
+      <c r="E6" s="6">
+        <v>33</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>907</v>
+      </c>
+      <c r="H6" s="7">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1490</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>613</v>
+      </c>
+      <c r="E7" s="6">
+        <v>38</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>908</v>
+      </c>
+      <c r="H7" s="7">
+        <v>3962</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1491</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>600</v>
+      </c>
+      <c r="E8" s="6">
+        <v>363</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>909</v>
+      </c>
+      <c r="H8" s="7">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="6">
+        <v>1492</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>633</v>
+      </c>
+      <c r="E9" s="6">
+        <v>27</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>910</v>
+      </c>
+      <c r="H9" s="7">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1494</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>662</v>
+      </c>
+      <c r="E10" s="6">
+        <v>1</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>911</v>
+      </c>
+      <c r="H10" s="7">
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="6">
+        <v>1495</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>657</v>
+      </c>
+      <c r="E11" s="6">
+        <v>2</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>912</v>
+      </c>
+      <c r="H11" s="7">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="6">
+        <v>1499</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>616</v>
+      </c>
+      <c r="E12" s="6">
+        <v>24</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>913</v>
+      </c>
+      <c r="H12" s="7">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1502</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>654</v>
+      </c>
+      <c r="E13" s="6">
+        <v>2</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>914</v>
+      </c>
+      <c r="H13" s="7">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1503</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>631</v>
+      </c>
+      <c r="E14" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1504</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>656</v>
+      </c>
+      <c r="E15" s="6">
+        <v>2</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="6">
+        <v>1505</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>648</v>
+      </c>
+      <c r="E16" s="6">
+        <v>12</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="6">
+        <v>1508</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>621</v>
+      </c>
+      <c r="E17" s="6">
+        <v>13</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>917</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>918</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>919</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>916</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="6">
+        <v>1512</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>611</v>
+      </c>
+      <c r="E18" s="6">
+        <v>16</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="6">
+        <v>1488</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="J18" s="6">
+        <v>144</v>
+      </c>
+      <c r="K18" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="6">
+        <v>1513</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="E19" s="6">
+        <v>1</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" s="6">
+        <v>1491</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>600</v>
+      </c>
+      <c r="J19" s="6">
+        <v>96</v>
+      </c>
+      <c r="K19" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1515</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>618</v>
+      </c>
+      <c r="E20" s="6">
+        <v>6</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="6">
+        <v>1499</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>616</v>
+      </c>
+      <c r="J20" s="6">
+        <v>29</v>
+      </c>
+      <c r="K20" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="6">
+        <v>1519</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>644</v>
+      </c>
+      <c r="E21" s="6">
+        <v>1</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="6">
+        <v>1503</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>631</v>
+      </c>
+      <c r="J21" s="6">
+        <v>3</v>
+      </c>
+      <c r="K21" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="6">
+        <v>1520</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>663</v>
+      </c>
+      <c r="E22" s="6">
+        <v>5</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" s="6">
+        <v>1508</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>621</v>
+      </c>
+      <c r="J22" s="6">
+        <v>13</v>
+      </c>
+      <c r="K22" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="6">
+        <v>1521</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>636</v>
+      </c>
+      <c r="E23" s="6">
+        <v>9</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" s="6">
+        <v>1512</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>611</v>
+      </c>
+      <c r="J23" s="6">
+        <v>42</v>
+      </c>
+      <c r="K23" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="6">
+        <v>1523</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>632</v>
+      </c>
+      <c r="E24" s="6">
+        <v>8</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H24" s="6">
+        <v>1513</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="J24" s="6">
+        <v>1</v>
+      </c>
+      <c r="K24" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="6">
+        <v>1524</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="E25" s="6">
+        <v>3</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" s="6">
+        <v>1515</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>618</v>
+      </c>
+      <c r="J25" s="6">
+        <v>85</v>
+      </c>
+      <c r="K25" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" s="6">
+        <v>1525</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>670</v>
+      </c>
+      <c r="E26" s="6">
+        <v>1</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" s="6">
+        <v>1524</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>655</v>
+      </c>
+      <c r="J26" s="6">
+        <v>1</v>
+      </c>
+      <c r="K26" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" s="6">
+        <v>1526</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>669</v>
+      </c>
+      <c r="E27" s="6">
+        <v>1</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" s="6">
+        <v>1529</v>
+      </c>
+      <c r="I27" s="6" t="s">
+        <v>615</v>
+      </c>
+      <c r="J27" s="6">
+        <v>1</v>
+      </c>
+      <c r="K27" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" s="6">
+        <v>1527</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>650</v>
+      </c>
+      <c r="E28" s="6">
+        <v>42</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H28" s="6">
+        <v>1533</v>
+      </c>
+      <c r="I28" s="6" t="s">
+        <v>603</v>
+      </c>
+      <c r="J28" s="6">
+        <v>19</v>
+      </c>
+      <c r="K28" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="6">
+        <v>1528</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>672</v>
+      </c>
+      <c r="E29" s="6">
+        <v>1</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H29" s="6">
+        <v>1537</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>643</v>
+      </c>
+      <c r="J29" s="6">
+        <v>11</v>
+      </c>
+      <c r="K29" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="6">
+        <v>1529</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>615</v>
+      </c>
+      <c r="E30" s="6">
+        <v>16</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H30" s="6">
+        <v>1538</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>604</v>
+      </c>
+      <c r="J30" s="6">
+        <v>49</v>
+      </c>
+      <c r="K30" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="6">
+        <v>1530</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>635</v>
+      </c>
+      <c r="E31" s="6">
+        <v>7</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H31" s="6">
+        <v>1539</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="J31" s="6">
+        <v>118</v>
+      </c>
+      <c r="K31" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="6">
+        <v>1531</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>664</v>
+      </c>
+      <c r="E32" s="6">
+        <v>6</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H32" s="6">
+        <v>1541</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>605</v>
+      </c>
+      <c r="J32" s="6">
+        <v>46</v>
+      </c>
+      <c r="K32" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="6">
+        <v>1532</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>638</v>
+      </c>
+      <c r="E33" s="6">
+        <v>5</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33" s="6">
+        <v>1544</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="J33" s="6">
+        <v>219</v>
+      </c>
+      <c r="K33" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="6">
+        <v>1533</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>603</v>
+      </c>
+      <c r="E34" s="6">
+        <v>136</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H34" s="6">
+        <v>1548</v>
+      </c>
+      <c r="I34" s="6" t="s">
+        <v>623</v>
+      </c>
+      <c r="J34" s="6">
+        <v>5</v>
+      </c>
+      <c r="K34" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="6">
+        <v>1535</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>622</v>
+      </c>
+      <c r="E35" s="6">
+        <v>9</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H35" s="6">
+        <v>1563</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>628</v>
+      </c>
+      <c r="J35" s="6">
+        <v>2</v>
+      </c>
+      <c r="K35" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" s="6">
+        <v>1537</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>643</v>
+      </c>
+      <c r="E36" s="6">
+        <v>9</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H36" s="6">
+        <v>1564</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>646</v>
+      </c>
+      <c r="J36" s="6">
+        <v>9</v>
+      </c>
+      <c r="K36" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="6">
+        <v>1538</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>604</v>
+      </c>
+      <c r="E37" s="6">
+        <v>13</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H37" s="6">
+        <v>1569</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>629</v>
+      </c>
+      <c r="J37" s="6">
+        <v>10</v>
+      </c>
+      <c r="K37" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="6">
+        <v>1539</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="E38" s="6">
+        <v>36</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H38" s="6">
+        <v>1571</v>
+      </c>
+      <c r="I38" s="6" t="s">
+        <v>606</v>
+      </c>
+      <c r="J38" s="6">
+        <v>89</v>
+      </c>
+      <c r="K38" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="6">
+        <v>1541</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>605</v>
+      </c>
+      <c r="E39" s="6">
+        <v>77</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H39" s="6">
+        <v>1573</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>645</v>
+      </c>
+      <c r="J39" s="6">
+        <v>3</v>
+      </c>
+      <c r="K39" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="6">
+        <v>1542</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>649</v>
+      </c>
+      <c r="E40" s="6">
+        <v>6</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H40" s="6">
+        <v>1575</v>
+      </c>
+      <c r="I40" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="J40" s="6">
+        <v>1</v>
+      </c>
+      <c r="K40" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="6">
+        <v>1544</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="E41" s="6">
+        <v>51</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H41" s="6">
+        <v>1582</v>
+      </c>
+      <c r="I41" s="6" t="s">
+        <v>651</v>
+      </c>
+      <c r="J41" s="6">
+        <v>13</v>
+      </c>
+      <c r="K41" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="6">
+        <v>1545</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>673</v>
+      </c>
+      <c r="E42" s="6">
+        <v>1</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H42" s="6">
+        <v>1583</v>
+      </c>
+      <c r="I42" s="6" t="s">
+        <v>634</v>
+      </c>
+      <c r="J42" s="6">
+        <v>7</v>
+      </c>
+      <c r="K42" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="6">
+        <v>1547</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>614</v>
+      </c>
+      <c r="E43" s="6">
+        <v>22</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H43" s="6">
+        <v>1585</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>609</v>
+      </c>
+      <c r="J43" s="6">
+        <v>14</v>
+      </c>
+      <c r="K43" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" s="6">
+        <v>1548</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>623</v>
+      </c>
+      <c r="E44" s="6">
+        <v>5</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H44" s="6">
+        <v>1590</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="J44" s="6">
+        <v>10</v>
+      </c>
+      <c r="K44" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="6">
+        <v>1549</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>612</v>
+      </c>
+      <c r="E45" s="6">
+        <v>54</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H45" s="6">
+        <v>1591</v>
+      </c>
+      <c r="I45" s="6" t="s">
+        <v>607</v>
+      </c>
+      <c r="J45" s="6">
+        <v>4</v>
+      </c>
+      <c r="K45" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" s="6">
+        <v>1552</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>676</v>
+      </c>
+      <c r="E46" s="6">
+        <v>2</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H46" s="6">
+        <v>1592</v>
+      </c>
+      <c r="I46" s="6" t="s">
+        <v>619</v>
+      </c>
+      <c r="J46" s="6">
+        <v>1</v>
+      </c>
+      <c r="K46" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="6">
+        <v>1553</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>626</v>
+      </c>
+      <c r="E47" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" s="6">
+        <v>1557</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>599</v>
+      </c>
+      <c r="E48" s="6">
+        <v>1</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="49" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="6">
+        <v>1558</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>658</v>
+      </c>
+      <c r="E49" s="6">
+        <v>3</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="50" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="6">
+        <v>1560</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>653</v>
+      </c>
+      <c r="E50" s="6">
+        <v>2</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>923</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>920</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>917</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>918</v>
+      </c>
+      <c r="K50" s="4" t="s">
+        <v>919</v>
+      </c>
+      <c r="L50" s="4" t="s">
+        <v>924</v>
+      </c>
+      <c r="M50" s="4" t="s">
+        <v>925</v>
+      </c>
+      <c r="N50" s="4" t="s">
+        <v>926</v>
+      </c>
+      <c r="O50" s="4" t="s">
+        <v>927</v>
+      </c>
+      <c r="P50" s="4" t="s">
+        <v>928</v>
+      </c>
+      <c r="Q50" s="4" t="s">
+        <v>929</v>
+      </c>
+      <c r="R50" s="4" t="s">
+        <v>930</v>
+      </c>
+      <c r="S50" s="4" t="s">
+        <v>931</v>
+      </c>
+      <c r="T50" s="4" t="s">
+        <v>932</v>
+      </c>
+      <c r="U50" s="4" t="s">
+        <v>936</v>
+      </c>
+      <c r="V50" s="4" t="s">
+        <v>937</v>
+      </c>
+      <c r="W50" s="4" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="51" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="6">
+        <v>1562</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>625</v>
+      </c>
+      <c r="E51" s="6">
+        <v>3</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>922</v>
+      </c>
+      <c r="H51" s="6">
+        <v>3</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J51" s="6">
+        <v>1529</v>
+      </c>
+      <c r="K51" s="6" t="s">
+        <v>615</v>
+      </c>
+      <c r="L51" s="6">
+        <v>12972503</v>
+      </c>
+      <c r="M51" s="6">
+        <v>3180561</v>
+      </c>
+      <c r="N51" s="6" t="s">
+        <v>714</v>
+      </c>
+      <c r="O51" s="6" t="s">
+        <v>715</v>
+      </c>
+      <c r="P51" s="6">
+        <v>3178549</v>
+      </c>
+      <c r="Q51" s="6">
+        <v>12713961</v>
+      </c>
+      <c r="R51" s="6" t="s">
+        <v>613</v>
+      </c>
+      <c r="S51" s="6">
+        <v>1490</v>
+      </c>
+      <c r="T51" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U51" s="6">
+        <v>1</v>
+      </c>
+      <c r="V51" s="6">
+        <v>1</v>
+      </c>
+      <c r="W51" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="6">
+        <v>1563</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>628</v>
+      </c>
+      <c r="E52" s="6">
+        <v>3</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>922</v>
+      </c>
+      <c r="H52" s="6">
+        <v>3</v>
+      </c>
+      <c r="I52" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J52" s="6">
+        <v>1539</v>
+      </c>
+      <c r="K52" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="L52" s="6">
+        <v>13024277</v>
+      </c>
+      <c r="M52" s="6">
+        <v>3181232</v>
+      </c>
+      <c r="N52" s="6" t="s">
+        <v>718</v>
+      </c>
+      <c r="O52" s="6" t="s">
+        <v>737</v>
+      </c>
+      <c r="P52" s="6">
+        <v>3180296</v>
+      </c>
+      <c r="Q52" s="6">
+        <v>12941639</v>
+      </c>
+      <c r="R52" s="6" t="s">
+        <v>611</v>
+      </c>
+      <c r="S52" s="6">
+        <v>1512</v>
+      </c>
+      <c r="T52" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U52" s="6">
+        <v>1</v>
+      </c>
+      <c r="V52" s="6">
+        <v>1</v>
+      </c>
+      <c r="W52" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="6">
+        <v>1564</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>646</v>
+      </c>
+      <c r="E53" s="6">
+        <v>3</v>
+      </c>
+      <c r="G53" s="6" t="s">
+        <v>922</v>
+      </c>
+      <c r="H53" s="6">
+        <v>3</v>
+      </c>
+      <c r="I53" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J53" s="6">
+        <v>1539</v>
+      </c>
+      <c r="K53" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="L53" s="6">
+        <v>13028676</v>
+      </c>
+      <c r="M53" s="6">
+        <v>3181315</v>
+      </c>
+      <c r="N53" s="6" t="s">
+        <v>721</v>
+      </c>
+      <c r="O53" s="6" t="s">
+        <v>737</v>
+      </c>
+      <c r="P53" s="6">
+        <v>3180296</v>
+      </c>
+      <c r="Q53" s="6">
+        <v>12941639</v>
+      </c>
+      <c r="R53" s="6" t="s">
+        <v>611</v>
+      </c>
+      <c r="S53" s="6">
+        <v>1512</v>
+      </c>
+      <c r="T53" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U53" s="6">
+        <v>1</v>
+      </c>
+      <c r="V53" s="6">
+        <v>1</v>
+      </c>
+      <c r="W53" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" s="6">
+        <v>1567</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>627</v>
+      </c>
+      <c r="E54" s="6">
+        <v>5</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>922</v>
+      </c>
+      <c r="H54" s="6">
+        <v>3</v>
+      </c>
+      <c r="I54" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J54" s="6">
+        <v>1541</v>
+      </c>
+      <c r="K54" s="6" t="s">
+        <v>605</v>
+      </c>
+      <c r="L54" s="6">
+        <v>13032743</v>
+      </c>
+      <c r="M54" s="6">
+        <v>3181490</v>
+      </c>
+      <c r="N54" s="6" t="s">
+        <v>738</v>
+      </c>
+      <c r="O54" s="6" t="s">
+        <v>737</v>
+      </c>
+      <c r="P54" s="6">
+        <v>3180296</v>
+      </c>
+      <c r="Q54" s="6">
+        <v>12941639</v>
+      </c>
+      <c r="R54" s="6" t="s">
+        <v>611</v>
+      </c>
+      <c r="S54" s="6">
+        <v>1512</v>
+      </c>
+      <c r="T54" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U54" s="6">
+        <v>1</v>
+      </c>
+      <c r="V54" s="6">
+        <v>1</v>
+      </c>
+      <c r="W54" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" s="6">
+        <v>1569</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>629</v>
+      </c>
+      <c r="E55" s="6">
+        <v>8</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>922</v>
+      </c>
+      <c r="H55" s="6">
+        <v>3</v>
+      </c>
+      <c r="I55" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J55" s="6">
+        <v>1541</v>
+      </c>
+      <c r="K55" s="6" t="s">
+        <v>605</v>
+      </c>
+      <c r="L55" s="6">
+        <v>13032743</v>
+      </c>
+      <c r="M55" s="6">
+        <v>3181490</v>
+      </c>
+      <c r="N55" s="6" t="s">
+        <v>738</v>
+      </c>
+      <c r="O55" s="6" t="s">
+        <v>718</v>
+      </c>
+      <c r="P55" s="6">
+        <v>3181232</v>
+      </c>
+      <c r="Q55" s="6">
+        <v>13024277</v>
+      </c>
+      <c r="R55" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="S55" s="6">
+        <v>1539</v>
+      </c>
+      <c r="T55" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U55" s="6">
+        <v>1</v>
+      </c>
+      <c r="V55" s="6">
+        <v>1</v>
+      </c>
+      <c r="W55" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" s="6">
+        <v>1571</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>606</v>
+      </c>
+      <c r="E56" s="6">
+        <v>14</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>922</v>
+      </c>
+      <c r="H56" s="6">
+        <v>3</v>
+      </c>
+      <c r="I56" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J56" s="6">
+        <v>1541</v>
+      </c>
+      <c r="K56" s="6" t="s">
+        <v>605</v>
+      </c>
+      <c r="L56" s="6">
+        <v>13032743</v>
+      </c>
+      <c r="M56" s="6">
+        <v>3181490</v>
+      </c>
+      <c r="N56" s="6" t="s">
+        <v>738</v>
+      </c>
+      <c r="O56" s="6" t="s">
+        <v>721</v>
+      </c>
+      <c r="P56" s="6">
+        <v>3181315</v>
+      </c>
+      <c r="Q56" s="6">
+        <v>13028676</v>
+      </c>
+      <c r="R56" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="S56" s="6">
+        <v>1539</v>
+      </c>
+      <c r="T56" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U56" s="6">
+        <v>1</v>
+      </c>
+      <c r="V56" s="6">
+        <v>1</v>
+      </c>
+      <c r="W56" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" s="6">
+        <v>1573</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>645</v>
+      </c>
+      <c r="E57" s="6">
+        <v>6</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>922</v>
+      </c>
+      <c r="H57" s="6">
+        <v>3</v>
+      </c>
+      <c r="I57" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J57" s="6">
+        <v>1544</v>
+      </c>
+      <c r="K57" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="L57" s="6">
+        <v>13039885</v>
+      </c>
+      <c r="M57" s="6">
+        <v>3181725</v>
+      </c>
+      <c r="N57" s="6" t="s">
+        <v>722</v>
+      </c>
+      <c r="O57" s="6" t="s">
+        <v>723</v>
+      </c>
+      <c r="P57" s="6">
+        <v>3178457</v>
+      </c>
+      <c r="Q57" s="6">
+        <v>12703956</v>
+      </c>
+      <c r="R57" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="S57" s="6">
+        <v>1488</v>
+      </c>
+      <c r="T57" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U57" s="6">
+        <v>1</v>
+      </c>
+      <c r="V57" s="6">
+        <v>1</v>
+      </c>
+      <c r="W57" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" s="6">
+        <v>1574</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>641</v>
+      </c>
+      <c r="E58" s="6">
+        <v>3</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>922</v>
+      </c>
+      <c r="H58" s="6">
+        <v>3</v>
+      </c>
+      <c r="I58" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J58" s="6">
+        <v>1544</v>
+      </c>
+      <c r="K58" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="L58" s="6">
+        <v>13039885</v>
+      </c>
+      <c r="M58" s="6">
+        <v>3181725</v>
+      </c>
+      <c r="N58" s="6" t="s">
+        <v>722</v>
+      </c>
+      <c r="O58" s="6" t="s">
+        <v>724</v>
+      </c>
+      <c r="P58" s="6">
+        <v>3178459</v>
+      </c>
+      <c r="Q58" s="6">
+        <v>12703958</v>
+      </c>
+      <c r="R58" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="S58" s="6">
+        <v>1488</v>
+      </c>
+      <c r="T58" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U58" s="6">
+        <v>1</v>
+      </c>
+      <c r="V58" s="6">
+        <v>1</v>
+      </c>
+      <c r="W58" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" s="6">
+        <v>1575</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>620</v>
+      </c>
+      <c r="E59" s="6">
+        <v>5</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>922</v>
+      </c>
+      <c r="H59" s="6">
+        <v>3</v>
+      </c>
+      <c r="I59" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J59" s="6">
+        <v>1544</v>
+      </c>
+      <c r="K59" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="L59" s="6">
+        <v>13039886</v>
+      </c>
+      <c r="M59" s="6">
+        <v>3181726</v>
+      </c>
+      <c r="N59" s="6" t="s">
+        <v>725</v>
+      </c>
+      <c r="O59" s="6" t="s">
+        <v>723</v>
+      </c>
+      <c r="P59" s="6">
+        <v>3178457</v>
+      </c>
+      <c r="Q59" s="6">
+        <v>12703956</v>
+      </c>
+      <c r="R59" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="S59" s="6">
+        <v>1488</v>
+      </c>
+      <c r="T59" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U59" s="6">
+        <v>1</v>
+      </c>
+      <c r="V59" s="6">
+        <v>1</v>
+      </c>
+      <c r="W59" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" s="6">
+        <v>1577</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>640</v>
+      </c>
+      <c r="E60" s="6">
+        <v>2</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>922</v>
+      </c>
+      <c r="H60" s="6">
+        <v>3</v>
+      </c>
+      <c r="I60" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J60" s="6">
+        <v>1544</v>
+      </c>
+      <c r="K60" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="L60" s="6">
+        <v>13039886</v>
+      </c>
+      <c r="M60" s="6">
+        <v>3181726</v>
+      </c>
+      <c r="N60" s="6" t="s">
+        <v>725</v>
+      </c>
+      <c r="O60" s="6" t="s">
+        <v>724</v>
+      </c>
+      <c r="P60" s="6">
+        <v>3178459</v>
+      </c>
+      <c r="Q60" s="6">
+        <v>12703958</v>
+      </c>
+      <c r="R60" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="S60" s="6">
+        <v>1488</v>
+      </c>
+      <c r="T60" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U60" s="6">
+        <v>1</v>
+      </c>
+      <c r="V60" s="6">
+        <v>1</v>
+      </c>
+      <c r="W60" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" s="6">
+        <v>1580</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>667</v>
+      </c>
+      <c r="E61" s="6">
+        <v>1</v>
+      </c>
+      <c r="G61" s="6" t="s">
+        <v>922</v>
+      </c>
+      <c r="H61" s="6">
+        <v>3</v>
+      </c>
+      <c r="I61" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J61" s="6">
+        <v>1544</v>
+      </c>
+      <c r="K61" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="L61" s="6">
+        <v>13039887</v>
+      </c>
+      <c r="M61" s="6">
+        <v>3181727</v>
+      </c>
+      <c r="N61" s="6" t="s">
+        <v>726</v>
+      </c>
+      <c r="O61" s="6" t="s">
+        <v>723</v>
+      </c>
+      <c r="P61" s="6">
+        <v>3178457</v>
+      </c>
+      <c r="Q61" s="6">
+        <v>12703956</v>
+      </c>
+      <c r="R61" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="S61" s="6">
+        <v>1488</v>
+      </c>
+      <c r="T61" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U61" s="6">
+        <v>1</v>
+      </c>
+      <c r="V61" s="6">
+        <v>1</v>
+      </c>
+      <c r="W61" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" s="6">
+        <v>1582</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>651</v>
+      </c>
+      <c r="E62" s="6">
+        <v>6</v>
+      </c>
+      <c r="G62" s="6" t="s">
+        <v>922</v>
+      </c>
+      <c r="H62" s="6">
+        <v>3</v>
+      </c>
+      <c r="I62" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J62" s="6">
+        <v>1544</v>
+      </c>
+      <c r="K62" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="L62" s="6">
+        <v>13039887</v>
+      </c>
+      <c r="M62" s="6">
+        <v>3181727</v>
+      </c>
+      <c r="N62" s="6" t="s">
+        <v>726</v>
+      </c>
+      <c r="O62" s="6" t="s">
+        <v>724</v>
+      </c>
+      <c r="P62" s="6">
+        <v>3178459</v>
+      </c>
+      <c r="Q62" s="6">
+        <v>12703958</v>
+      </c>
+      <c r="R62" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="S62" s="6">
+        <v>1488</v>
+      </c>
+      <c r="T62" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U62" s="6">
+        <v>1</v>
+      </c>
+      <c r="V62" s="6">
+        <v>1</v>
+      </c>
+      <c r="W62" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63" s="6">
+        <v>1583</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>634</v>
+      </c>
+      <c r="E63" s="6">
+        <v>19</v>
+      </c>
+      <c r="G63" s="6" t="s">
+        <v>922</v>
+      </c>
+      <c r="H63" s="6">
+        <v>3</v>
+      </c>
+      <c r="I63" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J63" s="6">
+        <v>1544</v>
+      </c>
+      <c r="K63" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="L63" s="6">
+        <v>13039888</v>
+      </c>
+      <c r="M63" s="6">
+        <v>3181728</v>
+      </c>
+      <c r="N63" s="6" t="s">
+        <v>727</v>
+      </c>
+      <c r="O63" s="6" t="s">
+        <v>723</v>
+      </c>
+      <c r="P63" s="6">
+        <v>3178457</v>
+      </c>
+      <c r="Q63" s="6">
+        <v>12703956</v>
+      </c>
+      <c r="R63" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="S63" s="6">
+        <v>1488</v>
+      </c>
+      <c r="T63" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U63" s="6">
+        <v>1</v>
+      </c>
+      <c r="V63" s="6">
+        <v>1</v>
+      </c>
+      <c r="W63" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" s="6">
+        <v>1585</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>609</v>
+      </c>
+      <c r="E64" s="6">
+        <v>98</v>
+      </c>
+      <c r="G64" s="6" t="s">
+        <v>922</v>
+      </c>
+      <c r="H64" s="6">
+        <v>3</v>
+      </c>
+      <c r="I64" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J64" s="6">
+        <v>1544</v>
+      </c>
+      <c r="K64" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="L64" s="6">
+        <v>13039888</v>
+      </c>
+      <c r="M64" s="6">
+        <v>3181728</v>
+      </c>
+      <c r="N64" s="6" t="s">
+        <v>727</v>
+      </c>
+      <c r="O64" s="6" t="s">
+        <v>724</v>
+      </c>
+      <c r="P64" s="6">
+        <v>3178459</v>
+      </c>
+      <c r="Q64" s="6">
+        <v>12703958</v>
+      </c>
+      <c r="R64" s="6" t="s">
+        <v>601</v>
+      </c>
+      <c r="S64" s="6">
+        <v>1488</v>
+      </c>
+      <c r="T64" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U64" s="6">
+        <v>1</v>
+      </c>
+      <c r="V64" s="6">
+        <v>1</v>
+      </c>
+      <c r="W64" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C65" s="6">
+        <v>1586</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>642</v>
+      </c>
+      <c r="E65" s="6">
+        <v>1</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>922</v>
+      </c>
+      <c r="H65" s="6">
+        <v>3</v>
+      </c>
+      <c r="I65" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J65" s="6">
+        <v>1563</v>
+      </c>
+      <c r="K65" s="6" t="s">
+        <v>628</v>
+      </c>
+      <c r="L65" s="6">
+        <v>13100428</v>
+      </c>
+      <c r="M65" s="6">
+        <v>3182722</v>
+      </c>
+      <c r="N65" s="6" t="s">
+        <v>745</v>
+      </c>
+      <c r="O65" s="6" t="s">
+        <v>746</v>
+      </c>
+      <c r="P65" s="6">
+        <v>3180306</v>
+      </c>
+      <c r="Q65" s="6">
+        <v>12943008</v>
+      </c>
+      <c r="R65" s="6" t="s">
+        <v>652</v>
+      </c>
+      <c r="S65" s="6">
+        <v>1513</v>
+      </c>
+      <c r="T65" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U65" s="6">
+        <v>1</v>
+      </c>
+      <c r="V65" s="6">
+        <v>1</v>
+      </c>
+      <c r="W65" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C66" s="6">
+        <v>1588</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>647</v>
+      </c>
+      <c r="E66" s="6">
+        <v>2</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>922</v>
+      </c>
+      <c r="H66" s="6">
+        <v>3</v>
+      </c>
+      <c r="I66" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J66" s="6">
+        <v>1569</v>
+      </c>
+      <c r="K66" s="6" t="s">
+        <v>629</v>
+      </c>
+      <c r="L66" s="6">
+        <v>13107187</v>
+      </c>
+      <c r="M66" s="6">
+        <v>3182799</v>
+      </c>
+      <c r="N66" s="6" t="s">
+        <v>739</v>
+      </c>
+      <c r="O66" s="6" t="s">
+        <v>740</v>
+      </c>
+      <c r="P66" s="6">
+        <v>3181942</v>
+      </c>
+      <c r="Q66" s="6">
+        <v>13045875</v>
+      </c>
+      <c r="R66" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="S66" s="6">
+        <v>1544</v>
+      </c>
+      <c r="T66" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U66" s="6">
+        <v>1</v>
+      </c>
+      <c r="V66" s="6">
+        <v>1</v>
+      </c>
+      <c r="W66" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C67" s="6">
+        <v>1590</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>617</v>
+      </c>
+      <c r="E67" s="6">
+        <v>3</v>
+      </c>
+      <c r="G67" s="6" t="s">
+        <v>922</v>
+      </c>
+      <c r="H67" s="6">
+        <v>3</v>
+      </c>
+      <c r="I67" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J67" s="6">
+        <v>1571</v>
+      </c>
+      <c r="K67" s="6" t="s">
+        <v>606</v>
+      </c>
+      <c r="L67" s="6">
+        <v>13113435</v>
+      </c>
+      <c r="M67" s="6">
+        <v>3182882</v>
+      </c>
+      <c r="N67" s="6" t="s">
+        <v>729</v>
+      </c>
+      <c r="O67" s="6" t="s">
+        <v>741</v>
+      </c>
+      <c r="P67" s="6">
+        <v>3181114</v>
+      </c>
+      <c r="Q67" s="6">
+        <v>13018324</v>
+      </c>
+      <c r="R67" s="6" t="s">
+        <v>643</v>
+      </c>
+      <c r="S67" s="6">
+        <v>1537</v>
+      </c>
+      <c r="T67" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U67" s="6">
+        <v>1</v>
+      </c>
+      <c r="V67" s="6">
+        <v>1</v>
+      </c>
+      <c r="W67" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68" s="6">
+        <v>1591</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>607</v>
+      </c>
+      <c r="E68" s="6">
+        <v>53</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>922</v>
+      </c>
+      <c r="H68" s="6">
+        <v>3</v>
+      </c>
+      <c r="I68" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J68" s="6">
+        <v>1582</v>
+      </c>
+      <c r="K68" s="6" t="s">
+        <v>651</v>
+      </c>
+      <c r="L68" s="6">
+        <v>13145550</v>
+      </c>
+      <c r="M68" s="6">
+        <v>3183462</v>
+      </c>
+      <c r="N68" s="6" t="s">
+        <v>728</v>
+      </c>
+      <c r="O68" s="6" t="s">
+        <v>741</v>
+      </c>
+      <c r="P68" s="6">
+        <v>3181114</v>
+      </c>
+      <c r="Q68" s="6">
+        <v>13018324</v>
+      </c>
+      <c r="R68" s="6" t="s">
+        <v>643</v>
+      </c>
+      <c r="S68" s="6">
+        <v>1537</v>
+      </c>
+      <c r="T68" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U68" s="6">
+        <v>1</v>
+      </c>
+      <c r="V68" s="6">
+        <v>1</v>
+      </c>
+      <c r="W68" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69" s="6">
+        <v>1592</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>619</v>
+      </c>
+      <c r="E69" s="6">
+        <v>25</v>
+      </c>
+      <c r="G69" s="6" t="s">
+        <v>922</v>
+      </c>
+      <c r="H69" s="6">
+        <v>3</v>
+      </c>
+      <c r="I69" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J69" s="6">
+        <v>1582</v>
+      </c>
+      <c r="K69" s="6" t="s">
+        <v>651</v>
+      </c>
+      <c r="L69" s="6">
+        <v>13145550</v>
+      </c>
+      <c r="M69" s="6">
+        <v>3183462</v>
+      </c>
+      <c r="N69" s="6" t="s">
+        <v>728</v>
+      </c>
+      <c r="O69" s="6" t="s">
+        <v>729</v>
+      </c>
+      <c r="P69" s="6">
+        <v>3182882</v>
+      </c>
+      <c r="Q69" s="6">
+        <v>13113435</v>
+      </c>
+      <c r="R69" s="6" t="s">
+        <v>606</v>
+      </c>
+      <c r="S69" s="6">
+        <v>1571</v>
+      </c>
+      <c r="T69" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U69" s="6">
+        <v>1</v>
+      </c>
+      <c r="V69" s="6">
+        <v>1</v>
+      </c>
+      <c r="W69" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C70" s="6">
+        <v>1594</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>665</v>
+      </c>
+      <c r="E70" s="6">
+        <v>6</v>
+      </c>
+      <c r="G70" s="6" t="s">
+        <v>922</v>
+      </c>
+      <c r="H70" s="6">
+        <v>3</v>
+      </c>
+      <c r="I70" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="J70" s="6">
+        <v>1591</v>
+      </c>
+      <c r="K70" s="6" t="s">
+        <v>607</v>
+      </c>
+      <c r="L70" s="6">
+        <v>13211380</v>
+      </c>
+      <c r="M70" s="6">
+        <v>3184224</v>
+      </c>
+      <c r="N70" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="O70" s="6" t="s">
+        <v>732</v>
+      </c>
+      <c r="P70" s="6">
+        <v>3180315</v>
+      </c>
+      <c r="Q70" s="6">
+        <v>12943813</v>
+      </c>
+      <c r="R70" s="6" t="s">
+        <v>618</v>
+      </c>
+      <c r="S70" s="6">
+        <v>1515</v>
+      </c>
+      <c r="T70" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="U70" s="6">
+        <v>1</v>
+      </c>
+      <c r="V70" s="6">
+        <v>1</v>
+      </c>
+      <c r="W70" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="2:23" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C71" s="6">
+        <v>1595</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>684</v>
+      </c>
+      <c r="E71" s="6">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:A182"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView showGridLines="0" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="A186" sqref="A186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12355,10 +15416,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F252"/>
+  <dimension ref="A1:F338"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A223" workbookViewId="0">
-      <selection activeCell="A220" sqref="A220:A253"/>
+    <sheetView showGridLines="0" topLeftCell="A314" workbookViewId="0">
+      <selection activeCell="A333" sqref="A333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13541,6 +16602,356 @@
         <v>472</v>
       </c>
     </row>
+    <row r="255" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A255" s="97" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="256" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A256" s="97" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="257" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A257" s="97" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="258" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A258" s="97" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="259" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A259" s="97" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="260" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A260" s="97" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="261" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A261" s="97" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="262" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A262" s="97" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="263" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A263" s="97" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="264" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A264" s="97" t="s">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="266" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A266" s="97" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="268" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A268" s="97" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="269" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A269" s="97" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="270" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A270" s="97" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="271" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A271" s="97" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="272" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A272" s="97" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="274" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A274" s="97" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="275" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A275" s="97" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="277" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A277" s="97" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="278" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A278" s="97" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="279" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A279" s="97" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="280" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A280" s="97" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="281" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A281" s="97" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="283" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A283" s="97" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="284" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A284" s="97" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="285" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A285" s="97" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="286" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A286" s="97" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="287" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A287" s="97" t="s">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="288" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A288" s="97" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="289" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A289" s="97" t="s">
+        <v>829</v>
+      </c>
+    </row>
+    <row r="291" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A291" s="97" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="292" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A292" s="97" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="293" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A293" s="97" t="s">
+        <v>832</v>
+      </c>
+    </row>
+    <row r="294" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A294" s="97" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="295" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A295" s="97" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="296" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A296" s="97" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="297" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A297" s="97" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="299" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A299" s="97" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="300" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A300" s="97" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="301" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A301" s="97" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A302" s="97" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="303" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A303" s="97" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="306" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A306" s="97" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="307" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A307" s="97" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="308" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A308" s="97" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="309" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A309" s="97" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="310" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A310" s="97" t="s">
+        <v>841</v>
+      </c>
+    </row>
+    <row r="311" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A311" s="97" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="312" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A312" s="97" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="313" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A313" s="97" t="s">
+        <v>843</v>
+      </c>
+    </row>
+    <row r="315" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A315" s="97" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="316" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A316" s="97" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="317" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A317" s="97" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A318" s="97" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A319" s="97" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A321" s="97" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A322" s="97" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A324" s="97" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A325" s="97" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="326" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A326" s="97" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A327" s="97" t="s">
+        <v>822</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A328" s="97" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A330" s="97" t="s">
+        <v>933</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A331" s="97" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A332" s="97" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A334" s="97" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A335" s="97" t="s">
+        <v>766</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A336" s="97" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A337" s="97" t="s">
+        <v>845</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A338" s="97" t="s">
+        <v>846</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -13548,10 +16959,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A316"/>
+  <dimension ref="A1:A427"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A278" workbookViewId="0">
-      <selection activeCell="A316" sqref="A286:A316"/>
+    <sheetView showGridLines="0" topLeftCell="A392" workbookViewId="0">
+      <selection activeCell="A402" sqref="A402"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15042,6 +18453,531 @@
     <row r="316" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A316" s="97" t="s">
         <v>772</v>
+      </c>
+    </row>
+    <row r="318" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A318" s="97" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="319" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A319" s="97" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="320" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A320" s="97" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="321" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A321" s="97" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="322" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A322" s="97" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="323" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A323" s="97" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="324" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A324" s="97" t="s">
+        <v>853</v>
+      </c>
+    </row>
+    <row r="325" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A325" s="97" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="327" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A327" s="97" t="s">
+        <v>855</v>
+      </c>
+    </row>
+    <row r="328" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A328" s="97" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="329" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A329" s="97" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="330" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A330" s="97" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="331" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A331" s="97" t="s">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="332" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A332" s="97" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="333" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A333" s="97" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="334" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A334" s="97" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="335" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A335" s="97" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="336" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A336" s="97" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A337" s="97" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A338" s="97" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A339" s="97" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="341" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A341" s="97" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="342" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A342" s="97" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="343" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A343" s="97" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="344" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A344" s="97" t="s">
+        <v>868</v>
+      </c>
+    </row>
+    <row r="345" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A345" s="97" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="346" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A346" s="97" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="347" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A347" s="97" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="348" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A348" s="97" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="349" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A349" s="97" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="350" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A350" s="97" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="351" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A351" s="97" t="s">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="352" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A352" s="97" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="353" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A353" s="97" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="354" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A354" s="97" t="s">
+        <v>862</v>
+      </c>
+    </row>
+    <row r="355" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A355" s="97" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="356" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A356" s="97" t="s">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="357" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A357" s="97" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A358" s="97" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A359" s="97" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A360" s="97" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A361" s="97" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="362" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A362" s="97" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="363" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A363" s="97" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="364" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A364" s="97" t="s">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="365" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A365" s="97" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="366" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A366" s="97" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="367" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A367" s="97" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="368" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A368" s="97" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="369" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A369" s="97" t="s">
+        <v>881</v>
+      </c>
+    </row>
+    <row r="370" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A370" s="97" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="371" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A371" s="97" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="372" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A372" s="97" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="373" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A373" s="97" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="374" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A374" s="97" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="375" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A375" s="97" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="376" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A376" s="97" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="377" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A377" s="97" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="378" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A378" s="97" t="s">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="379" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A379" s="97" t="s">
+        <v>884</v>
+      </c>
+    </row>
+    <row r="380" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A380" s="97" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="381" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A381" s="97" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="382" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A382" s="97" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="383" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A383" s="97" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="384" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A384" s="97" t="s">
+        <v>886</v>
+      </c>
+    </row>
+    <row r="385" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A385" s="97" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="386" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A386" s="97" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="387" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A387" s="97" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="388" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A388" s="97" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="389" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A389" s="97" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="390" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A390" s="97" t="s">
+        <v>890</v>
+      </c>
+    </row>
+    <row r="391" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A391" s="97" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="392" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A392" s="97" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="393" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A393" s="97" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="394" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A394" s="97" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="395" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A395" s="97" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="396" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A396" s="97" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="397" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A397" s="97" t="s">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="398" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A398" s="97" t="s">
+        <v>889</v>
+      </c>
+    </row>
+    <row r="400" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A400" s="97" t="s">
+        <v>893</v>
+      </c>
+    </row>
+    <row r="401" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A401" s="97" t="s">
+        <v>921</v>
+      </c>
+    </row>
+    <row r="402" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A402" s="97" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="403" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A403" s="97" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="404" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A404" s="97" t="s">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="405" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A405" s="97" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="406" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A406" s="97" t="s">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="407" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A407" s="97" t="s">
+        <v>877</v>
+      </c>
+    </row>
+    <row r="408" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A408" s="97" t="s">
+        <v>878</v>
+      </c>
+    </row>
+    <row r="409" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A409" s="97" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="410" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A410" s="97" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="411" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A411" s="97" t="s">
+        <v>895</v>
+      </c>
+    </row>
+    <row r="413" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A413" s="97" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="414" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A414" s="97" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="415" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A415" s="97" t="s">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="416" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A416" s="97" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="417" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A417" s="97" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="418" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A418" s="97" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="419" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A419" s="97" t="s">
+        <v>899</v>
+      </c>
+    </row>
+    <row r="421" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A421" s="97" t="s">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="422" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A422" s="97" t="s">
+        <v>901</v>
+      </c>
+    </row>
+    <row r="423" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A423" s="97" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="424" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A424" s="97" t="s">
+        <v>859</v>
+      </c>
+    </row>
+    <row r="425" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A425" s="97" t="s">
+        <v>887</v>
+      </c>
+    </row>
+    <row r="426" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A426" s="97" t="s">
+        <v>888</v>
+      </c>
+    </row>
+    <row r="427" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A427" s="97" t="s">
+        <v>903</v>
       </c>
     </row>
   </sheetData>
@@ -15056,8 +18992,8 @@
   </sheetPr>
   <dimension ref="B1:M59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -19381,7 +23317,7 @@
   <dimension ref="B1:L120"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A77" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A106" sqref="A106:XFD106"/>
+      <selection activeCell="B96" sqref="B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>

</xml_diff>